<commit_message>
FIxed wong parts number U1 - U4 as C86715
</commit_message>
<xml_diff>
--- a/Optinal Balanced Driver Board/JLPCB_OderFiles/BalancedDriverBoard_BOM1.xlsx
+++ b/Optinal Balanced Driver Board/JLPCB_OderFiles/BalancedDriverBoard_BOM1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/ADAU1701/FreeDSP_Catamaran/BalancedDriverBoard/JLPCB_OderFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{204DF446-DD55-0B4A-97EB-03076DA3198B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC15FE45-7FFF-8D46-B1F2-F08A22E0E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="4340" windowWidth="28300" windowHeight="17440"/>
+    <workbookView xWindow="440" yWindow="4040" windowWidth="28300" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BalancedDriverBoard_BOM1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="186">
   <si>
     <t xml:space="preserve">    C1</t>
   </si>
@@ -555,9 +555,6 @@
     <t xml:space="preserve">    U1</t>
   </si>
   <si>
-    <t>OPA1611</t>
-  </si>
-  <si>
     <t>Package_SO:SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
@@ -616,11 +613,26 @@
       <t>）</t>
     </r>
   </si>
+  <si>
+    <t>C86715</t>
+  </si>
+  <si>
+    <t>OPA1632DR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OPA1611AIDR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C86715</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -1036,11 +1048,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -1053,16 +1065,16 @@
   <sheetData>
     <row r="1" spans="1:16384">
       <c r="A1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
@@ -17447,72 +17459,72 @@
     </row>
     <row r="2" spans="1:16384">
       <c r="A2" s="4" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>171</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:16384">
       <c r="A3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:16384">
       <c r="A4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:16384">
       <c r="A5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:16384">
@@ -19152,7 +19164,7 @@
       <c r="D127" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XFD1">
+  <autoFilter ref="A1:XFD1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:XFD133">
       <sortCondition descending="1" ref="D1:D133"/>
     </sortState>

</xml_diff>

<commit_message>
Fixed wrong parts number U1 - U4 as C86715.
</commit_message>
<xml_diff>
--- a/Optinal Balanced Driver Board/JLPCB_OderFiles/BalancedDriverBoard_BOM1.xlsx
+++ b/Optinal Balanced Driver Board/JLPCB_OderFiles/BalancedDriverBoard_BOM1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/ADAU1701/FreeDSP_Catamaran/BalancedDriverBoard/JLPCB_OderFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC15FE45-7FFF-8D46-B1F2-F08A22E0E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F23C57-FF61-3240-BD79-47D74FA56DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="4040" windowWidth="28300" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,7 +633,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -667,6 +667,22 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -719,7 +735,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -733,6 +749,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1052,7 +1074,7 @@
   <dimension ref="A1:XFD127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="20"/>
@@ -17458,7 +17480,7 @@
       <c r="XFD1" s="2"/>
     </row>
     <row r="2" spans="1:16384">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -17467,12 +17489,12 @@
       <c r="C2" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:16384">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -17481,12 +17503,12 @@
       <c r="C3" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:16384">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -17495,12 +17517,12 @@
       <c r="C4" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:16384">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -17509,12 +17531,12 @@
       <c r="C5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:16384">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>184</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -17523,7 +17545,7 @@
       <c r="C6" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>